<commit_message>
add freeze in worksheet
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -33,7 +33,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +45,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,10 +93,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -134,7 +127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Batch 1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -160,301 +153,301 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.69937672963491</c:v>
+                  <c:v>68.60966037404884</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.88049100315784</c:v>
+                  <c:v>29.64592865212219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.32825101853283</c:v>
+                  <c:v>99.30783012513064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.01763946744937</c:v>
+                  <c:v>98.01277155162673</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.97075383266573</c:v>
+                  <c:v>10.56156501751727</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.58906189867574</c:v>
+                  <c:v>12.43269508403306</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.45706607755189</c:v>
+                  <c:v>30.05803620391759</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55.41255681517993</c:v>
+                  <c:v>84.25724272475</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76.46318718823449</c:v>
+                  <c:v>61.58163091631476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.67931028850435</c:v>
+                  <c:v>13.68817317312448</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.98567401664162</c:v>
+                  <c:v>62.6359066813536</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.406819939051</c:v>
+                  <c:v>60.94221763636764</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83.12055361325025</c:v>
+                  <c:v>40.62818569681687</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>93.38394294522369</c:v>
+                  <c:v>40.34272460823216</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>84.0703241085285</c:v>
+                  <c:v>43.0564913116247</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>57.18135493844682</c:v>
+                  <c:v>76.25013737341037</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70.84777631328267</c:v>
+                  <c:v>91.90029123199044</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>85.58356312103081</c:v>
+                  <c:v>55.01082657096406</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>58.86061344349162</c:v>
+                  <c:v>19.78285781970295</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17.1789196878305</c:v>
+                  <c:v>35.45985938824237</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>74.65896018630437</c:v>
+                  <c:v>91.29797588399498</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50.13824997666068</c:v>
+                  <c:v>63.86263436063707</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>98.95462808172329</c:v>
+                  <c:v>37.28936041526933</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30.5842401516426</c:v>
+                  <c:v>26.91120718948853</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>86.78564003245614</c:v>
+                  <c:v>15.95085227286263</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>66.98760625143524</c:v>
+                  <c:v>43.36226556338076</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86.3866111545878</c:v>
+                  <c:v>71.61509223803652</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>87.89244677979089</c:v>
+                  <c:v>70.59911065934618</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>28.11547218389643</c:v>
+                  <c:v>68.43768667576167</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>37.89085446029965</c:v>
+                  <c:v>21.33443310542808</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66.65247327905075</c:v>
+                  <c:v>74.82171111784254</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28.25020123935135</c:v>
+                  <c:v>78.98003773961912</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>75.74650205158299</c:v>
+                  <c:v>90.02341087777251</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>34.16920823132904</c:v>
+                  <c:v>98.05897068201891</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>62.55187120494409</c:v>
+                  <c:v>71.18483054944127</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>50.38324297908451</c:v>
+                  <c:v>80.54742775670195</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38.08525179778542</c:v>
+                  <c:v>17.6215699319453</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30.11539333237082</c:v>
+                  <c:v>84.5454747201137</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>65.40891874061087</c:v>
+                  <c:v>38.36308196035429</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>44.15112118951343</c:v>
+                  <c:v>40.34306353977752</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>94.34223026593781</c:v>
+                  <c:v>69.44183327396303</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>82.0452365808993</c:v>
+                  <c:v>53.43317962184632</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>98.2158887404448</c:v>
+                  <c:v>32.31766073408757</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>84.57007383224351</c:v>
+                  <c:v>87.16944731105117</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>28.30634935256842</c:v>
+                  <c:v>81.27480720404887</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>30.3845396979224</c:v>
+                  <c:v>84.15701981381237</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>98.32846864756388</c:v>
+                  <c:v>84.42081120224883</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>27.61862311889467</c:v>
+                  <c:v>86.68133465124829</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>63.89975826955598</c:v>
+                  <c:v>71.67224727410704</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.55212168555547</c:v>
+                  <c:v>89.98419380391204</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>22.13830686020021</c:v>
+                  <c:v>13.48911222983744</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>62.82219407787589</c:v>
+                  <c:v>69.45968840049585</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>55.6308331325931</c:v>
+                  <c:v>85.58007284393152</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>97.85462626322966</c:v>
+                  <c:v>30.68567531893252</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>71.07735413469867</c:v>
+                  <c:v>82.1353865958031</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>17.40546508997478</c:v>
+                  <c:v>83.73198638118075</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11.22633541342599</c:v>
+                  <c:v>54.10922834715919</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>71.75857687103309</c:v>
+                  <c:v>97.20698879854655</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>56.9107724013063</c:v>
+                  <c:v>71.06405034721172</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>41.47477450305941</c:v>
+                  <c:v>80.49342650973878</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42.82514113572447</c:v>
+                  <c:v>15.41650028238796</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>91.1431433955598</c:v>
+                  <c:v>15.75824804848915</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>51.74377392612084</c:v>
+                  <c:v>37.46682772785269</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>38.06794795275241</c:v>
+                  <c:v>98.94052097817737</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>80.86315420054748</c:v>
+                  <c:v>94.44283273796185</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>10.05850855450161</c:v>
+                  <c:v>25.72139139985678</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>51.58753254791964</c:v>
+                  <c:v>30.27815725792198</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>91.97109895340311</c:v>
+                  <c:v>13.85626395265158</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>93.84883575201893</c:v>
+                  <c:v>29.20912579357996</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>44.78400706481897</c:v>
+                  <c:v>71.45313050479862</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>80.88395812173677</c:v>
+                  <c:v>69.62257514910868</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>83.29337472833689</c:v>
+                  <c:v>13.36765835448523</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>69.39405668615105</c:v>
+                  <c:v>32.8404190708543</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>12.01935643146963</c:v>
+                  <c:v>89.02993026424228</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>33.35298738391277</c:v>
+                  <c:v>18.72759286905944</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>37.6118550004407</c:v>
+                  <c:v>56.19305276458238</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>75.38541815281447</c:v>
+                  <c:v>76.63119758027631</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>59.0607464908521</c:v>
+                  <c:v>22.2208611514948</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>63.52027195225843</c:v>
+                  <c:v>50.0411703587709</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>53.25468041329064</c:v>
+                  <c:v>13.13180923938958</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>91.97298409274342</c:v>
+                  <c:v>41.63540744354347</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>96.26350243543048</c:v>
+                  <c:v>87.90057723946444</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>53.3618661417859</c:v>
+                  <c:v>37.36371266812308</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>87.73527799318308</c:v>
+                  <c:v>75.34695289104954</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>82.18481486518682</c:v>
+                  <c:v>50.49804490816395</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>21.09081568532132</c:v>
+                  <c:v>12.67870795199642</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>37.1373539347405</c:v>
+                  <c:v>23.00433761220323</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>62.94537739699331</c:v>
+                  <c:v>87.74808961281212</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>37.41852063198462</c:v>
+                  <c:v>19.36882212444291</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>69.57648902348365</c:v>
+                  <c:v>29.53047767907153</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>31.48469477238967</c:v>
+                  <c:v>22.97826949831859</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>91.72278473146478</c:v>
+                  <c:v>42.54071588611612</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>23.19846758348954</c:v>
+                  <c:v>20.08850461184007</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>27.23048939996038</c:v>
+                  <c:v>50.7597801678674</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>82.26752450939006</c:v>
+                  <c:v>67.65237522137195</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>91.5395257005772</c:v>
+                  <c:v>19.13293828513796</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>24.93096678610969</c:v>
+                  <c:v>89.64156666404769</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>12.76905835068699</c:v>
+                  <c:v>65.48433467891617</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>50.43270643671538</c:v>
+                  <c:v>54.75687269224247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,7 +462,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Batch 2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -487,301 +480,301 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.32351749671892</c:v>
+                  <c:v>42.62395714004155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.59043903859323</c:v>
+                  <c:v>43.98390663145312</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.39735491120404</c:v>
+                  <c:v>32.37200629408105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.98971127865011</c:v>
+                  <c:v>36.46312576293139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.35575959584065</c:v>
+                  <c:v>49.16361718138103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.56571233306018</c:v>
+                  <c:v>45.0414252255642</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.74349197966676</c:v>
+                  <c:v>36.89791858084303</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.73047997963084</c:v>
+                  <c:v>43.63080031616366</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.47307291881778</c:v>
+                  <c:v>34.45124307432703</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.0926437417246</c:v>
+                  <c:v>25.41888599512477</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.31337712018382</c:v>
+                  <c:v>20.26623922069783</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.15572023421463</c:v>
+                  <c:v>20.57590371038324</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.05784028991505</c:v>
+                  <c:v>26.83872482719606</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.10640939756806</c:v>
+                  <c:v>26.61522227586713</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31.67957948711766</c:v>
+                  <c:v>43.41953316805605</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32.36722215317463</c:v>
+                  <c:v>21.63748265863266</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.4901201283147</c:v>
+                  <c:v>31.54888095677815</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.32516621551628</c:v>
+                  <c:v>47.3000961746756</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49.76260449226426</c:v>
+                  <c:v>36.28703484580373</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28.95237864834928</c:v>
+                  <c:v>41.83755428316373</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26.02059362639322</c:v>
+                  <c:v>48.63747513171319</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.07223526007333</c:v>
+                  <c:v>20.75878025871666</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46.66831482143404</c:v>
+                  <c:v>23.64365451343006</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30.57005576147951</c:v>
+                  <c:v>27.53872226607867</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39.37708483265504</c:v>
+                  <c:v>44.3603816265365</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21.53429846416705</c:v>
+                  <c:v>20.93985103728155</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26.56009755937174</c:v>
+                  <c:v>32.43366589204312</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>38.28852223142752</c:v>
+                  <c:v>21.49372940395521</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>31.06747854866153</c:v>
+                  <c:v>31.28792393418296</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25.56271862420945</c:v>
+                  <c:v>46.78342821049788</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41.72158751584436</c:v>
+                  <c:v>45.7557934344269</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41.89266495100822</c:v>
+                  <c:v>34.86252889919491</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>22.5238286613601</c:v>
+                  <c:v>26.01798811920965</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>26.96647858875153</c:v>
+                  <c:v>45.08314566856344</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35.11613960002817</c:v>
+                  <c:v>37.14426771099296</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41.66113865995591</c:v>
+                  <c:v>31.3125481578923</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>27.10272628694432</c:v>
+                  <c:v>23.18195399170667</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>48.60390942079331</c:v>
+                  <c:v>49.26914646425998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42.65326161136599</c:v>
+                  <c:v>25.89805744591756</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>22.25847174167748</c:v>
+                  <c:v>30.10876127203888</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>24.78162390434712</c:v>
+                  <c:v>41.29361663423967</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>40.97365566401493</c:v>
+                  <c:v>42.41023309609574</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>37.24112570738428</c:v>
+                  <c:v>31.59895017316055</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>38.08416466274306</c:v>
+                  <c:v>23.38366446044731</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>37.51183193294469</c:v>
+                  <c:v>23.38201145331303</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>34.87314885198666</c:v>
+                  <c:v>20.8650725951025</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>35.54821987651991</c:v>
+                  <c:v>37.13368368333187</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>30.8117625989488</c:v>
+                  <c:v>27.99141458227083</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>22.94954760145049</c:v>
+                  <c:v>42.97131066401221</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>44.06957843243036</c:v>
+                  <c:v>23.43473058445689</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>46.07375963906532</c:v>
+                  <c:v>35.27040563218181</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>35.21944047916285</c:v>
+                  <c:v>33.65998742484521</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>37.2242725327834</c:v>
+                  <c:v>22.64509139892418</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>21.19613835010363</c:v>
+                  <c:v>46.02033079739959</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>36.2230211392057</c:v>
+                  <c:v>32.4718787567905</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>43.94602261460444</c:v>
+                  <c:v>25.58561541243099</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>25.31478846089233</c:v>
+                  <c:v>38.82564435056884</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>21.0670677863061</c:v>
+                  <c:v>28.33661800814257</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>46.66233818596569</c:v>
+                  <c:v>36.58517677156686</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>38.71795616027429</c:v>
+                  <c:v>37.12968558758173</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42.75718004147608</c:v>
+                  <c:v>27.50849760142278</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>31.01193778487139</c:v>
+                  <c:v>38.78955167595831</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>46.72583266994989</c:v>
+                  <c:v>20.64960154819268</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>33.99804296537653</c:v>
+                  <c:v>49.64236922632684</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>49.22259676296645</c:v>
+                  <c:v>34.6165078185053</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>38.17830535042888</c:v>
+                  <c:v>44.87982928506753</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>28.99993659817905</c:v>
+                  <c:v>24.25999368816884</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>46.82998670524306</c:v>
+                  <c:v>49.47979851138874</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>41.2748268815048</c:v>
+                  <c:v>22.17161638308782</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>42.90476382257405</c:v>
+                  <c:v>23.41717703447151</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>47.5931515922525</c:v>
+                  <c:v>37.60682815895967</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>35.81266013900036</c:v>
+                  <c:v>24.53275998695528</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>43.6380467270385</c:v>
+                  <c:v>28.78836750735752</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>49.76755877396103</c:v>
+                  <c:v>25.04393401831031</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>41.5660933342122</c:v>
+                  <c:v>31.7398152704694</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>30.6380621254733</c:v>
+                  <c:v>24.03812918914274</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>42.87555082822938</c:v>
+                  <c:v>22.83911154199838</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>30.39421075114827</c:v>
+                  <c:v>30.02214852309255</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>31.4538070272948</c:v>
+                  <c:v>25.58419446707475</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>35.56427909343731</c:v>
+                  <c:v>28.36524563098796</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>38.04659974377612</c:v>
+                  <c:v>32.52356409383724</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>29.93742852408839</c:v>
+                  <c:v>21.35548383219962</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>36.69327371868724</c:v>
+                  <c:v>27.99740477454724</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>40.87822858841232</c:v>
+                  <c:v>46.35483361503537</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>40.47764663559587</c:v>
+                  <c:v>44.30863948382931</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>44.69772414562434</c:v>
+                  <c:v>21.69914143546837</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>27.28898156361082</c:v>
+                  <c:v>44.09060071804553</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>42.60781568095033</c:v>
+                  <c:v>28.80786820277745</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>31.22357892451548</c:v>
+                  <c:v>48.82695419092115</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>43.11513203959835</c:v>
+                  <c:v>39.04075292723662</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>31.02534310461225</c:v>
+                  <c:v>24.45937280951547</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>39.1557324611184</c:v>
+                  <c:v>23.32181323850114</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>30.88579634951858</c:v>
+                  <c:v>30.97073780368585</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>21.91031414349136</c:v>
+                  <c:v>24.88496621634372</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>24.90038595856405</c:v>
+                  <c:v>48.41019881168057</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>34.37866664678569</c:v>
+                  <c:v>29.60504151077456</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>39.04419492790517</c:v>
+                  <c:v>45.14383640474323</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>33.82071170696412</c:v>
+                  <c:v>22.93400340049954</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>25.46216079466463</c:v>
+                  <c:v>24.47206428903686</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1194,184 +1187,173 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>81.69937672963491</v>
+        <v>68.60966037404884</v>
       </c>
       <c r="C3" s="3">
-        <v>35.32351749671892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>42.62395714004155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>20.88049100315784</v>
+        <v>29.64592865212219</v>
       </c>
       <c r="C4" s="3">
-        <v>48.59043903859323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>43.98390663145312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>52.32825101853283</v>
+        <v>99.30783012513064</v>
       </c>
       <c r="C5" s="3">
-        <v>29.39735491120404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>32.37200629408105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>50.01763946744937</v>
+        <v>98.01277155162673</v>
       </c>
       <c r="C6" s="3">
-        <v>39.98971127865011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>36.46312576293139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>33.97075383266573</v>
+        <v>10.56156501751727</v>
       </c>
       <c r="C7" s="3">
-        <v>26.35575959584065</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>49.16361718138103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>14.58906189867574</v>
+        <v>12.43269508403306</v>
       </c>
       <c r="C8" s="3">
-        <v>45.56571233306018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>45.0414252255642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>14.45706607755189</v>
+        <v>30.05803620391759</v>
       </c>
       <c r="C9" s="3">
-        <v>36.74349197966676</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>36.89791858084303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>55.41255681517993</v>
+        <v>84.25724272475</v>
       </c>
       <c r="C10" s="3">
-        <v>30.73047997963084</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>43.63080031616366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>76.46318718823449</v>
+        <v>61.58163091631476</v>
       </c>
       <c r="C11" s="3">
-        <v>30.47307291881778</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>34.45124307432703</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>46.67931028850435</v>
+        <v>13.68817317312448</v>
       </c>
       <c r="C12" s="3">
-        <v>29.0926437417246</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>25.41888599512477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>50.98567401664162</v>
+        <v>62.6359066813536</v>
       </c>
       <c r="C13" s="3">
-        <v>34.31337712018382</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>20.26623922069783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>17.406819939051</v>
+        <v>60.94221763636764</v>
       </c>
       <c r="C14" s="3">
-        <v>38.15572023421463</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>20.57590371038324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>83.12055361325025</v>
+        <v>40.62818569681687</v>
       </c>
       <c r="C15" s="3">
-        <v>27.05784028991505</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>26.83872482719606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>93.38394294522369</v>
+        <v>40.34272460823216</v>
       </c>
       <c r="C16" s="3">
-        <v>35.10640939756806</v>
+        <v>26.61522227586713</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1379,10 +1361,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>84.0703241085285</v>
+        <v>43.0564913116247</v>
       </c>
       <c r="C17" s="3">
-        <v>31.67957948711766</v>
+        <v>43.41953316805605</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1390,10 +1372,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>57.18135493844682</v>
+        <v>76.25013737341037</v>
       </c>
       <c r="C18" s="3">
-        <v>32.36722215317463</v>
+        <v>21.63748265863266</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1401,10 +1383,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>70.84777631328267</v>
+        <v>91.90029123199044</v>
       </c>
       <c r="C19" s="3">
-        <v>30.4901201283147</v>
+        <v>31.54888095677815</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1412,10 +1394,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>85.58356312103081</v>
+        <v>55.01082657096406</v>
       </c>
       <c r="C20" s="3">
-        <v>29.32516621551628</v>
+        <v>47.3000961746756</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1423,10 +1405,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>58.86061344349162</v>
+        <v>19.78285781970295</v>
       </c>
       <c r="C21" s="3">
-        <v>49.76260449226426</v>
+        <v>36.28703484580373</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1434,10 +1416,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>17.1789196878305</v>
+        <v>35.45985938824237</v>
       </c>
       <c r="C22" s="3">
-        <v>28.95237864834928</v>
+        <v>41.83755428316373</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1445,10 +1427,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>74.65896018630437</v>
+        <v>91.29797588399498</v>
       </c>
       <c r="C23" s="3">
-        <v>26.02059362639322</v>
+        <v>48.63747513171319</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1456,10 +1438,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>50.13824997666068</v>
+        <v>63.86263436063707</v>
       </c>
       <c r="C24" s="3">
-        <v>20.07223526007333</v>
+        <v>20.75878025871666</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1467,10 +1449,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="3">
-        <v>98.95462808172329</v>
+        <v>37.28936041526933</v>
       </c>
       <c r="C25" s="3">
-        <v>46.66831482143404</v>
+        <v>23.64365451343006</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1478,10 +1460,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>30.5842401516426</v>
+        <v>26.91120718948853</v>
       </c>
       <c r="C26" s="3">
-        <v>30.57005576147951</v>
+        <v>27.53872226607867</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1489,10 +1471,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>86.78564003245614</v>
+        <v>15.95085227286263</v>
       </c>
       <c r="C27" s="3">
-        <v>39.37708483265504</v>
+        <v>44.3603816265365</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1500,10 +1482,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="3">
-        <v>66.98760625143524</v>
+        <v>43.36226556338076</v>
       </c>
       <c r="C28" s="3">
-        <v>21.53429846416705</v>
+        <v>20.93985103728155</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1511,10 +1493,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="3">
-        <v>86.3866111545878</v>
+        <v>71.61509223803652</v>
       </c>
       <c r="C29" s="3">
-        <v>26.56009755937174</v>
+        <v>32.43366589204312</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1522,10 +1504,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="3">
-        <v>87.89244677979089</v>
+        <v>70.59911065934618</v>
       </c>
       <c r="C30" s="3">
-        <v>38.28852223142752</v>
+        <v>21.49372940395521</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1533,10 +1515,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="3">
-        <v>28.11547218389643</v>
+        <v>68.43768667576167</v>
       </c>
       <c r="C31" s="3">
-        <v>31.06747854866153</v>
+        <v>31.28792393418296</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1544,10 +1526,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="3">
-        <v>37.89085446029965</v>
+        <v>21.33443310542808</v>
       </c>
       <c r="C32" s="3">
-        <v>25.56271862420945</v>
+        <v>46.78342821049788</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1555,10 +1537,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>66.65247327905075</v>
+        <v>74.82171111784254</v>
       </c>
       <c r="C33" s="3">
-        <v>41.72158751584436</v>
+        <v>45.7557934344269</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1566,10 +1548,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>28.25020123935135</v>
+        <v>78.98003773961912</v>
       </c>
       <c r="C34" s="3">
-        <v>41.89266495100822</v>
+        <v>34.86252889919491</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1577,10 +1559,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>75.74650205158299</v>
+        <v>90.02341087777251</v>
       </c>
       <c r="C35" s="3">
-        <v>22.5238286613601</v>
+        <v>26.01798811920965</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1588,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="3">
-        <v>34.16920823132904</v>
+        <v>98.05897068201891</v>
       </c>
       <c r="C36" s="3">
-        <v>26.96647858875153</v>
+        <v>45.08314566856344</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1599,10 +1581,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="3">
-        <v>62.55187120494409</v>
+        <v>71.18483054944127</v>
       </c>
       <c r="C37" s="3">
-        <v>35.11613960002817</v>
+        <v>37.14426771099296</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1610,10 +1592,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="3">
-        <v>50.38324297908451</v>
+        <v>80.54742775670195</v>
       </c>
       <c r="C38" s="3">
-        <v>41.66113865995591</v>
+        <v>31.3125481578923</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1621,10 +1603,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="3">
-        <v>38.08525179778542</v>
+        <v>17.6215699319453</v>
       </c>
       <c r="C39" s="3">
-        <v>27.10272628694432</v>
+        <v>23.18195399170667</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1632,10 +1614,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>30.11539333237082</v>
+        <v>84.5454747201137</v>
       </c>
       <c r="C40" s="3">
-        <v>48.60390942079331</v>
+        <v>49.26914646425998</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1643,10 +1625,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="3">
-        <v>65.40891874061087</v>
+        <v>38.36308196035429</v>
       </c>
       <c r="C41" s="3">
-        <v>42.65326161136599</v>
+        <v>25.89805744591756</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1654,10 +1636,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>44.15112118951343</v>
+        <v>40.34306353977752</v>
       </c>
       <c r="C42" s="3">
-        <v>22.25847174167748</v>
+        <v>30.10876127203888</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1665,10 +1647,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="3">
-        <v>94.34223026593781</v>
+        <v>69.44183327396303</v>
       </c>
       <c r="C43" s="3">
-        <v>24.78162390434712</v>
+        <v>41.29361663423967</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1676,10 +1658,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="3">
-        <v>82.0452365808993</v>
+        <v>53.43317962184632</v>
       </c>
       <c r="C44" s="3">
-        <v>40.97365566401493</v>
+        <v>42.41023309609574</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1687,10 +1669,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>98.2158887404448</v>
+        <v>32.31766073408757</v>
       </c>
       <c r="C45" s="3">
-        <v>37.24112570738428</v>
+        <v>31.59895017316055</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1698,10 +1680,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>84.57007383224351</v>
+        <v>87.16944731105117</v>
       </c>
       <c r="C46" s="3">
-        <v>38.08416466274306</v>
+        <v>23.38366446044731</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1709,10 +1691,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="3">
-        <v>28.30634935256842</v>
+        <v>81.27480720404887</v>
       </c>
       <c r="C47" s="3">
-        <v>37.51183193294469</v>
+        <v>23.38201145331303</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1720,10 +1702,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>30.3845396979224</v>
+        <v>84.15701981381237</v>
       </c>
       <c r="C48" s="3">
-        <v>34.87314885198666</v>
+        <v>20.8650725951025</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1731,10 +1713,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>98.32846864756388</v>
+        <v>84.42081120224883</v>
       </c>
       <c r="C49" s="3">
-        <v>35.54821987651991</v>
+        <v>37.13368368333187</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1742,10 +1724,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>27.61862311889467</v>
+        <v>86.68133465124829</v>
       </c>
       <c r="C50" s="3">
-        <v>30.8117625989488</v>
+        <v>27.99141458227083</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1753,10 +1735,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>63.89975826955598</v>
+        <v>71.67224727410704</v>
       </c>
       <c r="C51" s="3">
-        <v>22.94954760145049</v>
+        <v>42.97131066401221</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1764,10 +1746,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>50.55212168555547</v>
+        <v>89.98419380391204</v>
       </c>
       <c r="C52" s="3">
-        <v>44.06957843243036</v>
+        <v>23.43473058445689</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1775,10 +1757,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="3">
-        <v>22.13830686020021</v>
+        <v>13.48911222983744</v>
       </c>
       <c r="C53" s="3">
-        <v>46.07375963906532</v>
+        <v>35.27040563218181</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1786,10 +1768,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="3">
-        <v>62.82219407787589</v>
+        <v>69.45968840049585</v>
       </c>
       <c r="C54" s="3">
-        <v>35.21944047916285</v>
+        <v>33.65998742484521</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1797,10 +1779,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="3">
-        <v>55.6308331325931</v>
+        <v>85.58007284393152</v>
       </c>
       <c r="C55" s="3">
-        <v>37.2242725327834</v>
+        <v>22.64509139892418</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1808,10 +1790,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="3">
-        <v>97.85462626322966</v>
+        <v>30.68567531893252</v>
       </c>
       <c r="C56" s="3">
-        <v>21.19613835010363</v>
+        <v>46.02033079739959</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1819,10 +1801,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="3">
-        <v>71.07735413469867</v>
+        <v>82.1353865958031</v>
       </c>
       <c r="C57" s="3">
-        <v>36.2230211392057</v>
+        <v>32.4718787567905</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1830,10 +1812,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="3">
-        <v>17.40546508997478</v>
+        <v>83.73198638118075</v>
       </c>
       <c r="C58" s="3">
-        <v>43.94602261460444</v>
+        <v>25.58561541243099</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1841,10 +1823,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="3">
-        <v>11.22633541342599</v>
+        <v>54.10922834715919</v>
       </c>
       <c r="C59" s="3">
-        <v>25.31478846089233</v>
+        <v>38.82564435056884</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1852,10 +1834,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="3">
-        <v>71.75857687103309</v>
+        <v>97.20698879854655</v>
       </c>
       <c r="C60" s="3">
-        <v>21.0670677863061</v>
+        <v>28.33661800814257</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1863,10 +1845,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="3">
-        <v>56.9107724013063</v>
+        <v>71.06405034721172</v>
       </c>
       <c r="C61" s="3">
-        <v>46.66233818596569</v>
+        <v>36.58517677156686</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1874,10 +1856,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="3">
-        <v>41.47477450305941</v>
+        <v>80.49342650973878</v>
       </c>
       <c r="C62" s="3">
-        <v>38.71795616027429</v>
+        <v>37.12968558758173</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1885,10 +1867,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="3">
-        <v>42.82514113572447</v>
+        <v>15.41650028238796</v>
       </c>
       <c r="C63" s="3">
-        <v>42.75718004147608</v>
+        <v>27.50849760142278</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1896,10 +1878,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="3">
-        <v>91.1431433955598</v>
+        <v>15.75824804848915</v>
       </c>
       <c r="C64" s="3">
-        <v>31.01193778487139</v>
+        <v>38.78955167595831</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1907,10 +1889,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="3">
-        <v>51.74377392612084</v>
+        <v>37.46682772785269</v>
       </c>
       <c r="C65" s="3">
-        <v>46.72583266994989</v>
+        <v>20.64960154819268</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1918,10 +1900,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="3">
-        <v>38.06794795275241</v>
+        <v>98.94052097817737</v>
       </c>
       <c r="C66" s="3">
-        <v>33.99804296537653</v>
+        <v>49.64236922632684</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1929,10 +1911,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="3">
-        <v>80.86315420054748</v>
+        <v>94.44283273796185</v>
       </c>
       <c r="C67" s="3">
-        <v>49.22259676296645</v>
+        <v>34.6165078185053</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1940,10 +1922,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="3">
-        <v>10.05850855450161</v>
+        <v>25.72139139985678</v>
       </c>
       <c r="C68" s="3">
-        <v>38.17830535042888</v>
+        <v>44.87982928506753</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1951,10 +1933,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="3">
-        <v>51.58753254791964</v>
+        <v>30.27815725792198</v>
       </c>
       <c r="C69" s="3">
-        <v>28.99993659817905</v>
+        <v>24.25999368816884</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1962,10 +1944,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="3">
-        <v>91.97109895340311</v>
+        <v>13.85626395265158</v>
       </c>
       <c r="C70" s="3">
-        <v>46.82998670524306</v>
+        <v>49.47979851138874</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1973,10 +1955,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="3">
-        <v>93.84883575201893</v>
+        <v>29.20912579357996</v>
       </c>
       <c r="C71" s="3">
-        <v>41.2748268815048</v>
+        <v>22.17161638308782</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1984,10 +1966,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="3">
-        <v>44.78400706481897</v>
+        <v>71.45313050479862</v>
       </c>
       <c r="C72" s="3">
-        <v>42.90476382257405</v>
+        <v>23.41717703447151</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1995,10 +1977,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="3">
-        <v>80.88395812173677</v>
+        <v>69.62257514910868</v>
       </c>
       <c r="C73" s="3">
-        <v>47.5931515922525</v>
+        <v>37.60682815895967</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2006,10 +1988,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="3">
-        <v>83.29337472833689</v>
+        <v>13.36765835448523</v>
       </c>
       <c r="C74" s="3">
-        <v>35.81266013900036</v>
+        <v>24.53275998695528</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2017,10 +1999,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="3">
-        <v>69.39405668615105</v>
+        <v>32.8404190708543</v>
       </c>
       <c r="C75" s="3">
-        <v>43.6380467270385</v>
+        <v>28.78836750735752</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2028,10 +2010,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="3">
-        <v>12.01935643146963</v>
+        <v>89.02993026424228</v>
       </c>
       <c r="C76" s="3">
-        <v>49.76755877396103</v>
+        <v>25.04393401831031</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2039,10 +2021,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="3">
-        <v>33.35298738391277</v>
+        <v>18.72759286905944</v>
       </c>
       <c r="C77" s="3">
-        <v>41.5660933342122</v>
+        <v>31.7398152704694</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2050,10 +2032,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="3">
-        <v>37.6118550004407</v>
+        <v>56.19305276458238</v>
       </c>
       <c r="C78" s="3">
-        <v>30.6380621254733</v>
+        <v>24.03812918914274</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2061,10 +2043,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="3">
-        <v>75.38541815281447</v>
+        <v>76.63119758027631</v>
       </c>
       <c r="C79" s="3">
-        <v>42.87555082822938</v>
+        <v>22.83911154199838</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2072,10 +2054,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="3">
-        <v>59.0607464908521</v>
+        <v>22.2208611514948</v>
       </c>
       <c r="C80" s="3">
-        <v>30.39421075114827</v>
+        <v>30.02214852309255</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2083,10 +2065,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="3">
-        <v>63.52027195225843</v>
+        <v>50.0411703587709</v>
       </c>
       <c r="C81" s="3">
-        <v>31.4538070272948</v>
+        <v>25.58419446707475</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2094,10 +2076,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="3">
-        <v>53.25468041329064</v>
+        <v>13.13180923938958</v>
       </c>
       <c r="C82" s="3">
-        <v>35.56427909343731</v>
+        <v>28.36524563098796</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2105,10 +2087,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="3">
-        <v>91.97298409274342</v>
+        <v>41.63540744354347</v>
       </c>
       <c r="C83" s="3">
-        <v>38.04659974377612</v>
+        <v>32.52356409383724</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2116,10 +2098,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="3">
-        <v>96.26350243543048</v>
+        <v>87.90057723946444</v>
       </c>
       <c r="C84" s="3">
-        <v>29.93742852408839</v>
+        <v>21.35548383219962</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2127,10 +2109,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="3">
-        <v>53.3618661417859</v>
+        <v>37.36371266812308</v>
       </c>
       <c r="C85" s="3">
-        <v>36.69327371868724</v>
+        <v>27.99740477454724</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2138,10 +2120,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="3">
-        <v>87.73527799318308</v>
+        <v>75.34695289104954</v>
       </c>
       <c r="C86" s="3">
-        <v>40.87822858841232</v>
+        <v>46.35483361503537</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2149,10 +2131,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="3">
-        <v>82.18481486518682</v>
+        <v>50.49804490816395</v>
       </c>
       <c r="C87" s="3">
-        <v>40.47764663559587</v>
+        <v>44.30863948382931</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2160,10 +2142,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="3">
-        <v>21.09081568532132</v>
+        <v>12.67870795199642</v>
       </c>
       <c r="C88" s="3">
-        <v>44.69772414562434</v>
+        <v>21.69914143546837</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2171,10 +2153,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="3">
-        <v>37.1373539347405</v>
+        <v>23.00433761220323</v>
       </c>
       <c r="C89" s="3">
-        <v>27.28898156361082</v>
+        <v>44.09060071804553</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2182,10 +2164,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="3">
-        <v>62.94537739699331</v>
+        <v>87.74808961281212</v>
       </c>
       <c r="C90" s="3">
-        <v>42.60781568095033</v>
+        <v>28.80786820277745</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2193,10 +2175,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="3">
-        <v>37.41852063198462</v>
+        <v>19.36882212444291</v>
       </c>
       <c r="C91" s="3">
-        <v>31.22357892451548</v>
+        <v>48.82695419092115</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2204,10 +2186,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="3">
-        <v>69.57648902348365</v>
+        <v>29.53047767907153</v>
       </c>
       <c r="C92" s="3">
-        <v>43.11513203959835</v>
+        <v>39.04075292723662</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2215,10 +2197,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="3">
-        <v>31.48469477238967</v>
+        <v>22.97826949831859</v>
       </c>
       <c r="C93" s="3">
-        <v>31.02534310461225</v>
+        <v>24.45937280951547</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2226,10 +2208,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="3">
-        <v>91.72278473146478</v>
+        <v>42.54071588611612</v>
       </c>
       <c r="C94" s="3">
-        <v>39.1557324611184</v>
+        <v>23.32181323850114</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2237,10 +2219,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="3">
-        <v>23.19846758348954</v>
+        <v>20.08850461184007</v>
       </c>
       <c r="C95" s="3">
-        <v>30.88579634951858</v>
+        <v>30.97073780368585</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2248,10 +2230,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="3">
-        <v>27.23048939996038</v>
+        <v>50.7597801678674</v>
       </c>
       <c r="C96" s="3">
-        <v>21.91031414349136</v>
+        <v>24.88496621634372</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2259,10 +2241,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="3">
-        <v>82.26752450939006</v>
+        <v>67.65237522137195</v>
       </c>
       <c r="C97" s="3">
-        <v>24.90038595856405</v>
+        <v>48.41019881168057</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2270,10 +2252,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="3">
-        <v>91.5395257005772</v>
+        <v>19.13293828513796</v>
       </c>
       <c r="C98" s="3">
-        <v>34.37866664678569</v>
+        <v>29.60504151077456</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2281,10 +2263,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="3">
-        <v>24.93096678610969</v>
+        <v>89.64156666404769</v>
       </c>
       <c r="C99" s="3">
-        <v>39.04419492790517</v>
+        <v>45.14383640474323</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2292,10 +2274,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="3">
-        <v>12.76905835068699</v>
+        <v>65.48433467891617</v>
       </c>
       <c r="C100" s="3">
-        <v>33.82071170696412</v>
+        <v>22.93400340049954</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2303,10 +2285,10 @@
         <v>99</v>
       </c>
       <c r="B101" s="3">
-        <v>50.43270643671538</v>
+        <v>54.75687269224247</v>
       </c>
       <c r="C101" s="3">
-        <v>25.46216079466463</v>
+        <v>24.47206428903686</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2314,10 +2296,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="3">
-        <v>59.47873339196725</v>
+        <v>48.27727148077753</v>
       </c>
       <c r="C102" s="3">
-        <v>47.42860708406002</v>
+        <v>33.76548877584225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/06/01 headers & footers
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -195,301 +195,301 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.41412075116687</c:v>
+                  <c:v>39.23577335698774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.60577432838866</c:v>
+                  <c:v>72.63286427042766</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.86164982768997</c:v>
+                  <c:v>85.48944977156091</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.10819546828927</c:v>
+                  <c:v>66.27414717165985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63.82908239803041</c:v>
+                  <c:v>57.2292030243832</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.13544064450758</c:v>
+                  <c:v>81.21516868631056</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.86310839477903</c:v>
+                  <c:v>72.75954081781677</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>94.48320611846626</c:v>
+                  <c:v>67.10691517594549</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.69824666770874</c:v>
+                  <c:v>33.08534125355068</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>91.55620961387433</c:v>
+                  <c:v>84.19501281251148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.78253706071661</c:v>
+                  <c:v>21.18723951678372</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.75934627413885</c:v>
+                  <c:v>46.72077180121665</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>56.15501329933942</c:v>
+                  <c:v>41.30944801969044</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53.57238442290854</c:v>
+                  <c:v>91.06611566395077</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>91.43897129128207</c:v>
+                  <c:v>99.44301849449825</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>64.52006515001406</c:v>
+                  <c:v>76.41387318566319</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.65318517227427</c:v>
+                  <c:v>87.08676561992904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>80.71547237803348</c:v>
+                  <c:v>43.64581803335272</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48.92119824402967</c:v>
+                  <c:v>75.07158429322878</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34.39932692182817</c:v>
+                  <c:v>29.36747211147364</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>98.33135724503627</c:v>
+                  <c:v>86.03807922132282</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>54.82883459397822</c:v>
+                  <c:v>79.6352259360348</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25.7073872406811</c:v>
+                  <c:v>45.79773588904153</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.35705141999135</c:v>
+                  <c:v>30.82711705665798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>28.70460938511786</c:v>
+                  <c:v>98.15933428582757</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22.98766606747883</c:v>
+                  <c:v>17.79088403153667</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35.02669319566701</c:v>
+                  <c:v>81.94773652082075</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>65.57505777090424</c:v>
+                  <c:v>52.3012613198811</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>31.05835146002052</c:v>
+                  <c:v>57.76705934511367</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>85.98928913734376</c:v>
+                  <c:v>28.36984480130013</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41.10631464038931</c:v>
+                  <c:v>33.24156835964375</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>43.148350074906</c:v>
+                  <c:v>52.17883815289062</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>98.51337457495354</c:v>
+                  <c:v>99.45078309691065</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>82.66776467175059</c:v>
+                  <c:v>98.97000981774599</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>88.92917386827921</c:v>
+                  <c:v>92.77679089706085</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>63.3801328420361</c:v>
+                  <c:v>32.15435895003607</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>48.26747630574906</c:v>
+                  <c:v>26.31033094094217</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>88.49206632655904</c:v>
+                  <c:v>68.80863687596985</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>37.80926247621932</c:v>
+                  <c:v>24.57239170136759</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>37.26275589556938</c:v>
+                  <c:v>78.63197696252621</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>74.91213601594797</c:v>
+                  <c:v>73.58012591613694</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>31.6165898682456</c:v>
+                  <c:v>74.2664007906116</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>67.04405583483305</c:v>
+                  <c:v>24.55499502446218</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>87.04856714936163</c:v>
+                  <c:v>14.79394827326041</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17.10437657849702</c:v>
+                  <c:v>63.61967702743886</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>89.21197152763422</c:v>
+                  <c:v>49.14570799301205</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>65.62184915132931</c:v>
+                  <c:v>47.53312286378706</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>85.01080662013995</c:v>
+                  <c:v>18.94494359783769</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>96.88734424569662</c:v>
+                  <c:v>25.515722229359</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15.24630803519446</c:v>
+                  <c:v>31.77069605357499</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>69.27686106446912</c:v>
+                  <c:v>32.90011927135303</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>27.92181186681905</c:v>
+                  <c:v>33.06782993410243</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>96.43310225971372</c:v>
+                  <c:v>72.11066240882823</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>85.10661832200449</c:v>
+                  <c:v>18.30710781394842</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>58.22746212134533</c:v>
+                  <c:v>85.18471671809408</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>93.22123700918986</c:v>
+                  <c:v>17.76924925467925</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>74.75789317351305</c:v>
+                  <c:v>25.22775356497635</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>45.23290926661142</c:v>
+                  <c:v>25.6590116241461</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>60.41601511402811</c:v>
+                  <c:v>65.06902504046577</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>77.96809498895173</c:v>
+                  <c:v>84.15574674734648</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>65.34078159423765</c:v>
+                  <c:v>71.92361873116853</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>20.7098834135634</c:v>
+                  <c:v>61.11590107076167</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>51.46918279483572</c:v>
+                  <c:v>92.45551298503655</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>68.04748780438229</c:v>
+                  <c:v>52.31069226651419</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>66.55121123946293</c:v>
+                  <c:v>12.93560575858206</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>66.32398802887391</c:v>
+                  <c:v>83.48408408285165</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>41.81190575922527</c:v>
+                  <c:v>82.56645222691333</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>55.44928739336507</c:v>
+                  <c:v>82.75906502289928</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>47.57134140166727</c:v>
+                  <c:v>95.97865688784393</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>71.88168214230734</c:v>
+                  <c:v>31.96019631585754</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>84.94527735370484</c:v>
+                  <c:v>90.87687537356645</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>46.30009680049713</c:v>
+                  <c:v>55.75987911330556</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>82.25062356421014</c:v>
+                  <c:v>45.51763941169909</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>45.22017028672904</c:v>
+                  <c:v>14.29042509217282</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>13.31953595450318</c:v>
+                  <c:v>76.17623467420484</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>32.08805570836807</c:v>
+                  <c:v>75.44710850267617</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>75.13263231436133</c:v>
+                  <c:v>26.75451761951918</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>41.86510406680362</c:v>
+                  <c:v>59.66255752448487</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>61.8289816756105</c:v>
+                  <c:v>54.38090923712026</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>62.44348791533223</c:v>
+                  <c:v>30.89580250028337</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>36.89876136965296</c:v>
+                  <c:v>91.75111469592856</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>87.76967977561476</c:v>
+                  <c:v>10.4680778381256</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>99.62727575083916</c:v>
+                  <c:v>56.10115954983888</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>83.88200239211103</c:v>
+                  <c:v>20.29471488309852</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>25.53455234078083</c:v>
+                  <c:v>77.06430274114601</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>81.07460486078175</c:v>
+                  <c:v>75.78646766211354</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>14.22598457438631</c:v>
+                  <c:v>41.18284040293024</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>49.01703443424642</c:v>
+                  <c:v>24.68900822108959</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>74.85049957508537</c:v>
+                  <c:v>14.97319825809191</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>89.02064753963727</c:v>
+                  <c:v>41.77470635473715</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>61.49618711468226</c:v>
+                  <c:v>33.7577822330725</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>12.39080528749609</c:v>
+                  <c:v>35.95925633064175</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>44.83938569763383</c:v>
+                  <c:v>26.61164797653343</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>49.12720288395594</c:v>
+                  <c:v>90.60950945895202</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>99.44966630979218</c:v>
+                  <c:v>84.85104654073244</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>78.03935535127388</c:v>
+                  <c:v>58.38765191096734</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>15.93430327984005</c:v>
+                  <c:v>80.17905368822136</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>13.7737350655745</c:v>
+                  <c:v>75.82735267104459</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>60.61205298646618</c:v>
+                  <c:v>19.34325286952254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,301 +522,301 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.43736772945083</c:v>
+                  <c:v>47.04018127435583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.8666080715562</c:v>
+                  <c:v>42.18823360448647</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.0098534659312</c:v>
+                  <c:v>23.14312885621474</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.24982256404495</c:v>
+                  <c:v>46.62322222228221</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.79734256806742</c:v>
+                  <c:v>31.55686033938803</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.17640948390419</c:v>
+                  <c:v>20.72936827207329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.96485127944659</c:v>
+                  <c:v>20.08180396884948</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.19312959773364</c:v>
+                  <c:v>39.92294883566078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.95494453891558</c:v>
+                  <c:v>28.94569384900687</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44.4902096432379</c:v>
+                  <c:v>39.97081034356781</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.62176227303386</c:v>
+                  <c:v>38.49597365175428</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.29875536701547</c:v>
+                  <c:v>38.3279215307469</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.93141481235602</c:v>
+                  <c:v>35.74057748598389</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26.13932539828897</c:v>
+                  <c:v>46.23223490546113</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48.98218149376055</c:v>
+                  <c:v>27.94081876111392</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41.81924243481902</c:v>
+                  <c:v>24.24461985365533</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39.68323167812477</c:v>
+                  <c:v>44.56512519598101</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33.42095993706862</c:v>
+                  <c:v>24.03130894695769</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42.14185221231942</c:v>
+                  <c:v>47.42177104118579</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21.62283881861835</c:v>
+                  <c:v>48.25593746134354</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.2506357945379</c:v>
+                  <c:v>31.55723323540839</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.31804479188378</c:v>
+                  <c:v>40.32737443126655</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.4447060622322</c:v>
+                  <c:v>27.63845927973157</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27.75153514620848</c:v>
+                  <c:v>29.36642243333629</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.16740210817215</c:v>
+                  <c:v>22.31389116642872</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>39.28925655090516</c:v>
+                  <c:v>42.04875835987896</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35.97711382703811</c:v>
+                  <c:v>41.68085143190629</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35.1987009457011</c:v>
+                  <c:v>40.98314813143119</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44.21963973386097</c:v>
+                  <c:v>48.51142283063849</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44.33713497794149</c:v>
+                  <c:v>37.5423529742573</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>38.10214688250489</c:v>
+                  <c:v>23.28958550639066</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>45.40149935353156</c:v>
+                  <c:v>20.92365008687104</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30.52909785175164</c:v>
+                  <c:v>20.69627691745803</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>46.60067387685232</c:v>
+                  <c:v>25.51451589045954</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41.4853003773641</c:v>
+                  <c:v>33.26000973825369</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>23.94506701187959</c:v>
+                  <c:v>26.41481369817257</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21.53440175997565</c:v>
+                  <c:v>27.53140559713896</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>46.5310341799087</c:v>
+                  <c:v>44.07275859048771</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41.49630520223178</c:v>
+                  <c:v>29.57546019842502</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>21.61588730149817</c:v>
+                  <c:v>43.67222380401253</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>28.02741755691645</c:v>
+                  <c:v>26.05291692331841</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>23.65231198195699</c:v>
+                  <c:v>30.54460383841781</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44.33441388492212</c:v>
+                  <c:v>24.03136433009995</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>27.43844416014642</c:v>
+                  <c:v>27.87268538819498</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>36.46152276682773</c:v>
+                  <c:v>32.79120428066491</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>35.80825970841263</c:v>
+                  <c:v>26.34398742488648</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>44.27688573004824</c:v>
+                  <c:v>36.12039835334564</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>27.21325543635639</c:v>
+                  <c:v>37.14826115252241</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49.91720004482544</c:v>
+                  <c:v>33.05296055167679</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>45.45173293704691</c:v>
+                  <c:v>37.56292079189016</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>44.37965340181504</c:v>
+                  <c:v>41.02086270083907</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>22.67455971896079</c:v>
+                  <c:v>46.65877912510312</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>37.86169714211749</c:v>
+                  <c:v>31.3512497033985</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41.79614382112379</c:v>
+                  <c:v>49.13616891651313</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>46.89542685644493</c:v>
+                  <c:v>31.51760823921753</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>21.99079707538657</c:v>
+                  <c:v>21.99056507950483</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>34.63212647589994</c:v>
+                  <c:v>27.86162783882427</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>39.30768734859186</c:v>
+                  <c:v>40.72039143072105</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>35.72392732089682</c:v>
+                  <c:v>37.31452479111872</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42.52372826937928</c:v>
+                  <c:v>37.52239868435721</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>46.92147864995712</c:v>
+                  <c:v>26.20801921078083</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>31.49823780244953</c:v>
+                  <c:v>42.31163977917407</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>26.34478368462304</c:v>
+                  <c:v>42.09420288963406</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>22.24634606716904</c:v>
+                  <c:v>26.76025746879534</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>34.54135777330647</c:v>
+                  <c:v>28.08062625651204</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24.91467105670048</c:v>
+                  <c:v>33.28972417799283</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>49.17131261283389</c:v>
+                  <c:v>28.67752361455787</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>25.04089706142801</c:v>
+                  <c:v>40.46897422822042</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>48.54890248068621</c:v>
+                  <c:v>24.78545660990291</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>49.54804613482372</c:v>
+                  <c:v>43.94552396500203</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>37.95210486755072</c:v>
+                  <c:v>49.12870721054803</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>34.1171560540112</c:v>
+                  <c:v>27.10783829409558</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>30.22715493226665</c:v>
+                  <c:v>27.55779915452553</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>38.2721325496727</c:v>
+                  <c:v>46.60188675812946</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>40.05589640766648</c:v>
+                  <c:v>28.81752394603479</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>43.00910658446792</c:v>
+                  <c:v>44.81301561795043</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>33.51692995754623</c:v>
+                  <c:v>23.22758894871619</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>45.92028414179168</c:v>
+                  <c:v>36.23844869686091</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>23.65158504235312</c:v>
+                  <c:v>45.54772395871676</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>24.26487995069563</c:v>
+                  <c:v>28.52781043465851</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>31.62333390781066</c:v>
+                  <c:v>31.85163714677044</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>27.30605170733878</c:v>
+                  <c:v>42.17751393174115</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>34.55615294939682</c:v>
+                  <c:v>21.48219699532644</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>21.1936237938373</c:v>
+                  <c:v>27.57302724979548</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>30.96942667715138</c:v>
+                  <c:v>41.69351192645295</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>38.06282141275959</c:v>
+                  <c:v>43.8542624843478</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>33.39906205074502</c:v>
+                  <c:v>36.12807706212911</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>29.81896251083168</c:v>
+                  <c:v>26.73469467363554</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>24.08727260751641</c:v>
+                  <c:v>21.58491406660707</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>23.61009558259297</c:v>
+                  <c:v>33.77357401021008</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>37.91019310956415</c:v>
+                  <c:v>42.04054714039459</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>34.29258704921702</c:v>
+                  <c:v>22.34742493671132</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>38.81170240616618</c:v>
+                  <c:v>40.47026304634029</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>49.81545448714261</c:v>
+                  <c:v>37.63761255728356</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>33.073543082788</c:v>
+                  <c:v>40.77656780218561</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>20.35187289214509</c:v>
+                  <c:v>39.39373129558659</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>30.60112970670375</c:v>
+                  <c:v>49.01158066030919</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>36.30119695524621</c:v>
+                  <c:v>33.96058242001801</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>20.72427378240467</c:v>
+                  <c:v>25.05445152693918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1261,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <v>44713.15238124723</v>
+        <v>44714.07562935339</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1272,10 +1272,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>17.41412075116687</v>
+        <v>39.23577335698774</v>
       </c>
       <c r="C3" s="5">
-        <v>45.43736772945083</v>
+        <v>47.04018127435583</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25" customHeight="1">
@@ -1283,10 +1283,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>54.60577432838866</v>
+        <v>72.63286427042766</v>
       </c>
       <c r="C4" s="5">
-        <v>45.8666080715562</v>
+        <v>42.18823360448647</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25" customHeight="1">
@@ -1294,10 +1294,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>32.86164982768997</v>
+        <v>85.48944977156091</v>
       </c>
       <c r="C5" s="5">
-        <v>24.0098534659312</v>
+        <v>23.14312885621474</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25" customHeight="1">
@@ -1305,10 +1305,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>45.10819546828927</v>
+        <v>66.27414717165985</v>
       </c>
       <c r="C6" s="5">
-        <v>41.24982256404495</v>
+        <v>46.62322222228221</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25" customHeight="1">
@@ -1316,10 +1316,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>63.82908239803041</v>
+        <v>57.2292030243832</v>
       </c>
       <c r="C7" s="5">
-        <v>34.79734256806742</v>
+        <v>31.55686033938803</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25" customHeight="1">
@@ -1327,10 +1327,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <v>20.13544064450758</v>
+        <v>81.21516868631056</v>
       </c>
       <c r="C8" s="5">
-        <v>41.17640948390419</v>
+        <v>20.72936827207329</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25" customHeight="1">
@@ -1338,10 +1338,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5">
-        <v>21.86310839477903</v>
+        <v>72.75954081781677</v>
       </c>
       <c r="C9" s="5">
-        <v>42.96485127944659</v>
+        <v>20.08180396884948</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25" customHeight="1">
@@ -1349,10 +1349,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>94.48320611846626</v>
+        <v>67.10691517594549</v>
       </c>
       <c r="C10" s="5">
-        <v>28.19312959773364</v>
+        <v>39.92294883566078</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25" customHeight="1">
@@ -1360,10 +1360,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <v>80.69824666770874</v>
+        <v>33.08534125355068</v>
       </c>
       <c r="C11" s="5">
-        <v>38.95494453891558</v>
+        <v>28.94569384900687</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25" customHeight="1">
@@ -1371,10 +1371,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>91.55620961387433</v>
+        <v>84.19501281251148</v>
       </c>
       <c r="C12" s="5">
-        <v>44.4902096432379</v>
+        <v>39.97081034356781</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25" customHeight="1">
@@ -1382,10 +1382,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <v>97.78253706071661</v>
+        <v>21.18723951678372</v>
       </c>
       <c r="C13" s="5">
-        <v>20.62176227303386</v>
+        <v>38.49597365175428</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25" customHeight="1">
@@ -1393,10 +1393,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>11.75934627413885</v>
+        <v>46.72077180121665</v>
       </c>
       <c r="C14" s="5">
-        <v>34.29875536701547</v>
+        <v>38.3279215307469</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25" customHeight="1">
@@ -1404,10 +1404,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>56.15501329933942</v>
+        <v>41.30944801969044</v>
       </c>
       <c r="C15" s="5">
-        <v>34.93141481235602</v>
+        <v>35.74057748598389</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25" customHeight="1">
@@ -1415,10 +1415,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>53.57238442290854</v>
+        <v>91.06611566395077</v>
       </c>
       <c r="C16" s="5">
-        <v>26.13932539828897</v>
+        <v>46.23223490546113</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="25" customHeight="1">
@@ -1426,10 +1426,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>91.43897129128207</v>
+        <v>99.44301849449825</v>
       </c>
       <c r="C17" s="5">
-        <v>48.98218149376055</v>
+        <v>27.94081876111392</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="25" customHeight="1">
@@ -1437,10 +1437,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>64.52006515001406</v>
+        <v>76.41387318566319</v>
       </c>
       <c r="C18" s="5">
-        <v>41.81924243481902</v>
+        <v>24.24461985365533</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="25" customHeight="1">
@@ -1448,10 +1448,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>17.65318517227427</v>
+        <v>87.08676561992904</v>
       </c>
       <c r="C19" s="5">
-        <v>39.68323167812477</v>
+        <v>44.56512519598101</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="25" customHeight="1">
@@ -1459,10 +1459,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>80.71547237803348</v>
+        <v>43.64581803335272</v>
       </c>
       <c r="C20" s="5">
-        <v>33.42095993706862</v>
+        <v>24.03130894695769</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="25" customHeight="1">
@@ -1470,10 +1470,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>48.92119824402967</v>
+        <v>75.07158429322878</v>
       </c>
       <c r="C21" s="5">
-        <v>42.14185221231942</v>
+        <v>47.42177104118579</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="25" customHeight="1">
@@ -1481,10 +1481,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <v>34.39932692182817</v>
+        <v>29.36747211147364</v>
       </c>
       <c r="C22" s="5">
-        <v>21.62283881861835</v>
+        <v>48.25593746134354</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="25" customHeight="1">
@@ -1492,10 +1492,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="5">
-        <v>98.33135724503627</v>
+        <v>86.03807922132282</v>
       </c>
       <c r="C23" s="5">
-        <v>36.2506357945379</v>
+        <v>31.55723323540839</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="25" customHeight="1">
@@ -1503,10 +1503,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>54.82883459397822</v>
+        <v>79.6352259360348</v>
       </c>
       <c r="C24" s="5">
-        <v>32.31804479188378</v>
+        <v>40.32737443126655</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="25" customHeight="1">
@@ -1514,10 +1514,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>25.7073872406811</v>
+        <v>45.79773588904153</v>
       </c>
       <c r="C25" s="5">
-        <v>21.4447060622322</v>
+        <v>27.63845927973157</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="25" customHeight="1">
@@ -1525,10 +1525,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="5">
-        <v>13.35705141999135</v>
+        <v>30.82711705665798</v>
       </c>
       <c r="C26" s="5">
-        <v>27.75153514620848</v>
+        <v>29.36642243333629</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="25" customHeight="1">
@@ -1536,10 +1536,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="5">
-        <v>28.70460938511786</v>
+        <v>98.15933428582757</v>
       </c>
       <c r="C27" s="5">
-        <v>23.16740210817215</v>
+        <v>22.31389116642872</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="25" customHeight="1">
@@ -1547,10 +1547,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="5">
-        <v>22.98766606747883</v>
+        <v>17.79088403153667</v>
       </c>
       <c r="C28" s="5">
-        <v>39.28925655090516</v>
+        <v>42.04875835987896</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="25" customHeight="1">
@@ -1558,10 +1558,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="5">
-        <v>35.02669319566701</v>
+        <v>81.94773652082075</v>
       </c>
       <c r="C29" s="5">
-        <v>35.97711382703811</v>
+        <v>41.68085143190629</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="25" customHeight="1">
@@ -1569,10 +1569,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="5">
-        <v>65.57505777090424</v>
+        <v>52.3012613198811</v>
       </c>
       <c r="C30" s="5">
-        <v>35.1987009457011</v>
+        <v>40.98314813143119</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="25" customHeight="1">
@@ -1580,10 +1580,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="5">
-        <v>31.05835146002052</v>
+        <v>57.76705934511367</v>
       </c>
       <c r="C31" s="5">
-        <v>44.21963973386097</v>
+        <v>48.51142283063849</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="25" customHeight="1">
@@ -1591,10 +1591,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>85.98928913734376</v>
+        <v>28.36984480130013</v>
       </c>
       <c r="C32" s="5">
-        <v>44.33713497794149</v>
+        <v>37.5423529742573</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="25" customHeight="1">
@@ -1602,10 +1602,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="5">
-        <v>41.10631464038931</v>
+        <v>33.24156835964375</v>
       </c>
       <c r="C33" s="5">
-        <v>38.10214688250489</v>
+        <v>23.28958550639066</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="25" customHeight="1">
@@ -1613,10 +1613,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="5">
-        <v>43.148350074906</v>
+        <v>52.17883815289062</v>
       </c>
       <c r="C34" s="5">
-        <v>45.40149935353156</v>
+        <v>20.92365008687104</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="25" customHeight="1">
@@ -1624,10 +1624,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="5">
-        <v>98.51337457495354</v>
+        <v>99.45078309691065</v>
       </c>
       <c r="C35" s="5">
-        <v>30.52909785175164</v>
+        <v>20.69627691745803</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="25" customHeight="1">
@@ -1635,10 +1635,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="5">
-        <v>82.66776467175059</v>
+        <v>98.97000981774599</v>
       </c>
       <c r="C36" s="5">
-        <v>46.60067387685232</v>
+        <v>25.51451589045954</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="25" customHeight="1">
@@ -1646,10 +1646,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="5">
-        <v>88.92917386827921</v>
+        <v>92.77679089706085</v>
       </c>
       <c r="C37" s="5">
-        <v>41.4853003773641</v>
+        <v>33.26000973825369</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="25" customHeight="1">
@@ -1657,10 +1657,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="5">
-        <v>63.3801328420361</v>
+        <v>32.15435895003607</v>
       </c>
       <c r="C38" s="5">
-        <v>23.94506701187959</v>
+        <v>26.41481369817257</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="25" customHeight="1">
@@ -1668,10 +1668,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="5">
-        <v>48.26747630574906</v>
+        <v>26.31033094094217</v>
       </c>
       <c r="C39" s="5">
-        <v>21.53440175997565</v>
+        <v>27.53140559713896</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="25" customHeight="1">
@@ -1679,10 +1679,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="5">
-        <v>88.49206632655904</v>
+        <v>68.80863687596985</v>
       </c>
       <c r="C40" s="5">
-        <v>46.5310341799087</v>
+        <v>44.07275859048771</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="25" customHeight="1">
@@ -1690,10 +1690,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="5">
-        <v>37.80926247621932</v>
+        <v>24.57239170136759</v>
       </c>
       <c r="C41" s="5">
-        <v>41.49630520223178</v>
+        <v>29.57546019842502</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="25" customHeight="1">
@@ -1701,10 +1701,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="5">
-        <v>37.26275589556938</v>
+        <v>78.63197696252621</v>
       </c>
       <c r="C42" s="5">
-        <v>21.61588730149817</v>
+        <v>43.67222380401253</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="25" customHeight="1">
@@ -1712,10 +1712,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="5">
-        <v>74.91213601594797</v>
+        <v>73.58012591613694</v>
       </c>
       <c r="C43" s="5">
-        <v>28.02741755691645</v>
+        <v>26.05291692331841</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="25" customHeight="1">
@@ -1723,10 +1723,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="5">
-        <v>31.6165898682456</v>
+        <v>74.2664007906116</v>
       </c>
       <c r="C44" s="5">
-        <v>23.65231198195699</v>
+        <v>30.54460383841781</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="25" customHeight="1">
@@ -1734,10 +1734,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="5">
-        <v>67.04405583483305</v>
+        <v>24.55499502446218</v>
       </c>
       <c r="C45" s="5">
-        <v>44.33441388492212</v>
+        <v>24.03136433009995</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="25" customHeight="1">
@@ -1745,10 +1745,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="5">
-        <v>87.04856714936163</v>
+        <v>14.79394827326041</v>
       </c>
       <c r="C46" s="5">
-        <v>27.43844416014642</v>
+        <v>27.87268538819498</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="25" customHeight="1">
@@ -1756,10 +1756,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="5">
-        <v>17.10437657849702</v>
+        <v>63.61967702743886</v>
       </c>
       <c r="C47" s="5">
-        <v>36.46152276682773</v>
+        <v>32.79120428066491</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="25" customHeight="1">
@@ -1767,10 +1767,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="5">
-        <v>89.21197152763422</v>
+        <v>49.14570799301205</v>
       </c>
       <c r="C48" s="5">
-        <v>35.80825970841263</v>
+        <v>26.34398742488648</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="25" customHeight="1">
@@ -1778,10 +1778,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="5">
-        <v>65.62184915132931</v>
+        <v>47.53312286378706</v>
       </c>
       <c r="C49" s="5">
-        <v>44.27688573004824</v>
+        <v>36.12039835334564</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="25" customHeight="1">
@@ -1789,10 +1789,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="5">
-        <v>85.01080662013995</v>
+        <v>18.94494359783769</v>
       </c>
       <c r="C50" s="5">
-        <v>27.21325543635639</v>
+        <v>37.14826115252241</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="25" customHeight="1">
@@ -1800,10 +1800,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="5">
-        <v>96.88734424569662</v>
+        <v>25.515722229359</v>
       </c>
       <c r="C51" s="5">
-        <v>49.91720004482544</v>
+        <v>33.05296055167679</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="25" customHeight="1">
@@ -1811,10 +1811,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="5">
-        <v>15.24630803519446</v>
+        <v>31.77069605357499</v>
       </c>
       <c r="C52" s="5">
-        <v>45.45173293704691</v>
+        <v>37.56292079189016</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="25" customHeight="1">
@@ -1822,10 +1822,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="5">
-        <v>69.27686106446912</v>
+        <v>32.90011927135303</v>
       </c>
       <c r="C53" s="5">
-        <v>44.37965340181504</v>
+        <v>41.02086270083907</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="25" customHeight="1">
@@ -1833,10 +1833,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="5">
-        <v>27.92181186681905</v>
+        <v>33.06782993410243</v>
       </c>
       <c r="C54" s="5">
-        <v>22.67455971896079</v>
+        <v>46.65877912510312</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="25" customHeight="1">
@@ -1844,10 +1844,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="5">
-        <v>96.43310225971372</v>
+        <v>72.11066240882823</v>
       </c>
       <c r="C55" s="5">
-        <v>37.86169714211749</v>
+        <v>31.3512497033985</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="25" customHeight="1">
@@ -1855,10 +1855,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="5">
-        <v>85.10661832200449</v>
+        <v>18.30710781394842</v>
       </c>
       <c r="C56" s="5">
-        <v>41.79614382112379</v>
+        <v>49.13616891651313</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="25" customHeight="1">
@@ -1866,10 +1866,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="5">
-        <v>58.22746212134533</v>
+        <v>85.18471671809408</v>
       </c>
       <c r="C57" s="5">
-        <v>46.89542685644493</v>
+        <v>31.51760823921753</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="25" customHeight="1">
@@ -1877,10 +1877,10 @@
         <v>56</v>
       </c>
       <c r="B58" s="5">
-        <v>93.22123700918986</v>
+        <v>17.76924925467925</v>
       </c>
       <c r="C58" s="5">
-        <v>21.99079707538657</v>
+        <v>21.99056507950483</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="25" customHeight="1">
@@ -1888,10 +1888,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="5">
-        <v>74.75789317351305</v>
+        <v>25.22775356497635</v>
       </c>
       <c r="C59" s="5">
-        <v>34.63212647589994</v>
+        <v>27.86162783882427</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="25" customHeight="1">
@@ -1899,10 +1899,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="5">
-        <v>45.23290926661142</v>
+        <v>25.6590116241461</v>
       </c>
       <c r="C60" s="5">
-        <v>39.30768734859186</v>
+        <v>40.72039143072105</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="25" customHeight="1">
@@ -1910,10 +1910,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="5">
-        <v>60.41601511402811</v>
+        <v>65.06902504046577</v>
       </c>
       <c r="C61" s="5">
-        <v>35.72392732089682</v>
+        <v>37.31452479111872</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="25" customHeight="1">
@@ -1921,10 +1921,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="5">
-        <v>77.96809498895173</v>
+        <v>84.15574674734648</v>
       </c>
       <c r="C62" s="5">
-        <v>42.52372826937928</v>
+        <v>37.52239868435721</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="25" customHeight="1">
@@ -1932,10 +1932,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="5">
-        <v>65.34078159423765</v>
+        <v>71.92361873116853</v>
       </c>
       <c r="C63" s="5">
-        <v>46.92147864995712</v>
+        <v>26.20801921078083</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="25" customHeight="1">
@@ -1943,10 +1943,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="5">
-        <v>20.7098834135634</v>
+        <v>61.11590107076167</v>
       </c>
       <c r="C64" s="5">
-        <v>31.49823780244953</v>
+        <v>42.31163977917407</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="25" customHeight="1">
@@ -1954,10 +1954,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="5">
-        <v>51.46918279483572</v>
+        <v>92.45551298503655</v>
       </c>
       <c r="C65" s="5">
-        <v>26.34478368462304</v>
+        <v>42.09420288963406</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="25" customHeight="1">
@@ -1965,10 +1965,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="5">
-        <v>68.04748780438229</v>
+        <v>52.31069226651419</v>
       </c>
       <c r="C66" s="5">
-        <v>22.24634606716904</v>
+        <v>26.76025746879534</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="25" customHeight="1">
@@ -1976,10 +1976,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="5">
-        <v>66.55121123946293</v>
+        <v>12.93560575858206</v>
       </c>
       <c r="C67" s="5">
-        <v>34.54135777330647</v>
+        <v>28.08062625651204</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="25" customHeight="1">
@@ -1987,10 +1987,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="5">
-        <v>66.32398802887391</v>
+        <v>83.48408408285165</v>
       </c>
       <c r="C68" s="5">
-        <v>24.91467105670048</v>
+        <v>33.28972417799283</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="25" customHeight="1">
@@ -1998,10 +1998,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="5">
-        <v>41.81190575922527</v>
+        <v>82.56645222691333</v>
       </c>
       <c r="C69" s="5">
-        <v>49.17131261283389</v>
+        <v>28.67752361455787</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="25" customHeight="1">
@@ -2009,10 +2009,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="5">
-        <v>55.44928739336507</v>
+        <v>82.75906502289928</v>
       </c>
       <c r="C70" s="5">
-        <v>25.04089706142801</v>
+        <v>40.46897422822042</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="25" customHeight="1">
@@ -2020,10 +2020,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="5">
-        <v>47.57134140166727</v>
+        <v>95.97865688784393</v>
       </c>
       <c r="C71" s="5">
-        <v>48.54890248068621</v>
+        <v>24.78545660990291</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="25" customHeight="1">
@@ -2031,10 +2031,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="5">
-        <v>71.88168214230734</v>
+        <v>31.96019631585754</v>
       </c>
       <c r="C72" s="5">
-        <v>49.54804613482372</v>
+        <v>43.94552396500203</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="25" customHeight="1">
@@ -2042,10 +2042,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="5">
-        <v>84.94527735370484</v>
+        <v>90.87687537356645</v>
       </c>
       <c r="C73" s="5">
-        <v>37.95210486755072</v>
+        <v>49.12870721054803</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="25" customHeight="1">
@@ -2053,10 +2053,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="5">
-        <v>46.30009680049713</v>
+        <v>55.75987911330556</v>
       </c>
       <c r="C74" s="5">
-        <v>34.1171560540112</v>
+        <v>27.10783829409558</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="25" customHeight="1">
@@ -2064,10 +2064,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="5">
-        <v>82.25062356421014</v>
+        <v>45.51763941169909</v>
       </c>
       <c r="C75" s="5">
-        <v>30.22715493226665</v>
+        <v>27.55779915452553</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="25" customHeight="1">
@@ -2075,10 +2075,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="5">
-        <v>45.22017028672904</v>
+        <v>14.29042509217282</v>
       </c>
       <c r="C76" s="5">
-        <v>38.2721325496727</v>
+        <v>46.60188675812946</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="25" customHeight="1">
@@ -2086,10 +2086,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="5">
-        <v>13.31953595450318</v>
+        <v>76.17623467420484</v>
       </c>
       <c r="C77" s="5">
-        <v>40.05589640766648</v>
+        <v>28.81752394603479</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="25" customHeight="1">
@@ -2097,10 +2097,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="5">
-        <v>32.08805570836807</v>
+        <v>75.44710850267617</v>
       </c>
       <c r="C78" s="5">
-        <v>43.00910658446792</v>
+        <v>44.81301561795043</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="25" customHeight="1">
@@ -2108,10 +2108,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="5">
-        <v>75.13263231436133</v>
+        <v>26.75451761951918</v>
       </c>
       <c r="C79" s="5">
-        <v>33.51692995754623</v>
+        <v>23.22758894871619</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="25" customHeight="1">
@@ -2119,10 +2119,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="5">
-        <v>41.86510406680362</v>
+        <v>59.66255752448487</v>
       </c>
       <c r="C80" s="5">
-        <v>45.92028414179168</v>
+        <v>36.23844869686091</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="25" customHeight="1">
@@ -2130,10 +2130,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="5">
-        <v>61.8289816756105</v>
+        <v>54.38090923712026</v>
       </c>
       <c r="C81" s="5">
-        <v>23.65158504235312</v>
+        <v>45.54772395871676</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="25" customHeight="1">
@@ -2141,10 +2141,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="5">
-        <v>62.44348791533223</v>
+        <v>30.89580250028337</v>
       </c>
       <c r="C82" s="5">
-        <v>24.26487995069563</v>
+        <v>28.52781043465851</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="25" customHeight="1">
@@ -2152,10 +2152,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="5">
-        <v>36.89876136965296</v>
+        <v>91.75111469592856</v>
       </c>
       <c r="C83" s="5">
-        <v>31.62333390781066</v>
+        <v>31.85163714677044</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="25" customHeight="1">
@@ -2163,10 +2163,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="5">
-        <v>87.76967977561476</v>
+        <v>10.4680778381256</v>
       </c>
       <c r="C84" s="5">
-        <v>27.30605170733878</v>
+        <v>42.17751393174115</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="25" customHeight="1">
@@ -2174,10 +2174,10 @@
         <v>83</v>
       </c>
       <c r="B85" s="5">
-        <v>99.62727575083916</v>
+        <v>56.10115954983888</v>
       </c>
       <c r="C85" s="5">
-        <v>34.55615294939682</v>
+        <v>21.48219699532644</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="25" customHeight="1">
@@ -2185,10 +2185,10 @@
         <v>84</v>
       </c>
       <c r="B86" s="5">
-        <v>83.88200239211103</v>
+        <v>20.29471488309852</v>
       </c>
       <c r="C86" s="5">
-        <v>21.1936237938373</v>
+        <v>27.57302724979548</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="25" customHeight="1">
@@ -2196,10 +2196,10 @@
         <v>85</v>
       </c>
       <c r="B87" s="5">
-        <v>25.53455234078083</v>
+        <v>77.06430274114601</v>
       </c>
       <c r="C87" s="5">
-        <v>30.96942667715138</v>
+        <v>41.69351192645295</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="25" customHeight="1">
@@ -2207,10 +2207,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="5">
-        <v>81.07460486078175</v>
+        <v>75.78646766211354</v>
       </c>
       <c r="C88" s="5">
-        <v>38.06282141275959</v>
+        <v>43.8542624843478</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="25" customHeight="1">
@@ -2218,10 +2218,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="5">
-        <v>14.22598457438631</v>
+        <v>41.18284040293024</v>
       </c>
       <c r="C89" s="5">
-        <v>33.39906205074502</v>
+        <v>36.12807706212911</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="25" customHeight="1">
@@ -2229,10 +2229,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="5">
-        <v>49.01703443424642</v>
+        <v>24.68900822108959</v>
       </c>
       <c r="C90" s="5">
-        <v>29.81896251083168</v>
+        <v>26.73469467363554</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="25" customHeight="1">
@@ -2240,10 +2240,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="5">
-        <v>74.85049957508537</v>
+        <v>14.97319825809191</v>
       </c>
       <c r="C91" s="5">
-        <v>24.08727260751641</v>
+        <v>21.58491406660707</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="25" customHeight="1">
@@ -2251,10 +2251,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="5">
-        <v>89.02064753963727</v>
+        <v>41.77470635473715</v>
       </c>
       <c r="C92" s="5">
-        <v>23.61009558259297</v>
+        <v>33.77357401021008</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="25" customHeight="1">
@@ -2262,10 +2262,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="5">
-        <v>61.49618711468226</v>
+        <v>33.7577822330725</v>
       </c>
       <c r="C93" s="5">
-        <v>37.91019310956415</v>
+        <v>42.04054714039459</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="25" customHeight="1">
@@ -2273,10 +2273,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="5">
-        <v>12.39080528749609</v>
+        <v>35.95925633064175</v>
       </c>
       <c r="C94" s="5">
-        <v>34.29258704921702</v>
+        <v>22.34742493671132</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="25" customHeight="1">
@@ -2284,10 +2284,10 @@
         <v>93</v>
       </c>
       <c r="B95" s="5">
-        <v>44.83938569763383</v>
+        <v>26.61164797653343</v>
       </c>
       <c r="C95" s="5">
-        <v>38.81170240616618</v>
+        <v>40.47026304634029</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="25" customHeight="1">
@@ -2295,10 +2295,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="5">
-        <v>49.12720288395594</v>
+        <v>90.60950945895202</v>
       </c>
       <c r="C96" s="5">
-        <v>49.81545448714261</v>
+        <v>37.63761255728356</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="25" customHeight="1">
@@ -2306,10 +2306,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="5">
-        <v>99.44966630979218</v>
+        <v>84.85104654073244</v>
       </c>
       <c r="C97" s="5">
-        <v>33.073543082788</v>
+        <v>40.77656780218561</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="25" customHeight="1">
@@ -2317,10 +2317,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="5">
-        <v>78.03935535127388</v>
+        <v>58.38765191096734</v>
       </c>
       <c r="C98" s="5">
-        <v>20.35187289214509</v>
+        <v>39.39373129558659</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="25" customHeight="1">
@@ -2328,10 +2328,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="5">
-        <v>15.93430327984005</v>
+        <v>80.17905368822136</v>
       </c>
       <c r="C99" s="5">
-        <v>30.60112970670375</v>
+        <v>49.01158066030919</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="25" customHeight="1">
@@ -2339,10 +2339,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="5">
-        <v>13.7737350655745</v>
+        <v>75.82735267104459</v>
       </c>
       <c r="C100" s="5">
-        <v>36.30119695524621</v>
+        <v>33.96058242001801</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="25" customHeight="1">
@@ -2350,10 +2350,10 @@
         <v>99</v>
       </c>
       <c r="B101" s="5">
-        <v>60.61205298646618</v>
+        <v>19.34325286952254</v>
       </c>
       <c r="C101" s="5">
-        <v>20.72427378240467</v>
+        <v>25.05445152693918</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="25" customHeight="1">
@@ -2361,10 +2361,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="5">
-        <v>60.92513752710239</v>
+        <v>32.85927714800223</v>
       </c>
       <c r="C102" s="5">
-        <v>29.31457584859837</v>
+        <v>33.49646907467381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>